<commit_message>
Final Commit. Added Maven Surefire and Compile Plugins and run.bat file
</commit_message>
<xml_diff>
--- a/testData/Opencart_LoginData.xlsx
+++ b/testData/Opencart_LoginData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\burha\eclipse-workspace\opencart_autV1\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C3E5398-BC05-46BD-9B7E-8CF924861AFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A82910-B1C1-4D3A-AA00-A2329E1507E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{1F2D179E-37D2-4BC0-88A9-F5C135B87DA5}"/>
+    <workbookView xWindow="3240" yWindow="3045" windowWidth="15375" windowHeight="7875" xr2:uid="{1F2D179E-37D2-4BC0-88A9-F5C135B87DA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,31 +45,31 @@
     <t>Valid</t>
   </si>
   <si>
-    <t>laksh@yahoo.com</t>
-  </si>
-  <si>
     <t>Laxmi</t>
   </si>
   <si>
     <t>Invalid</t>
   </si>
   <si>
-    <t>laks@yahoo.com</t>
-  </si>
-  <si>
     <t>xyz</t>
   </si>
   <si>
     <t>test@123</t>
   </si>
   <si>
-    <t>abc123@gmail.com</t>
-  </si>
-  <si>
     <t>slatke@gmail.com</t>
   </si>
   <si>
     <t>Rebo123@</t>
+  </si>
+  <si>
+    <t>ahmet@yahoo.com</t>
+  </si>
+  <si>
+    <t>firat@gmail.com</t>
+  </si>
+  <si>
+    <t>burcu@yahoo.com</t>
   </si>
 </sst>
 </file>
@@ -467,7 +467,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,10 +490,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>5</v>
@@ -504,7 +504,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>5</v>
@@ -512,7 +512,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>4</v>
@@ -523,24 +523,24 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>